<commit_message>
02. Play with Docker Classrom
</commit_message>
<xml_diff>
--- a/00. Huong dan Docker.xlsx
+++ b/00. Huong dan Docker.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
     <sheet name="01" sheetId="2" r:id="rId2"/>
-    <sheet name="02" sheetId="3" r:id="rId3"/>
+    <sheet name="02" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>Sharing Docker dành cho Liên - Hiếu - Thảo</t>
   </si>
@@ -115,12 +115,49 @@
   <si>
     <t>https://blogs.technet.microsoft.com/canitpro/2015/09/08/step-by-step-enabling-hyper-v-for-use-on-windows-10/</t>
   </si>
+  <si>
+    <t>02. Play With Docker Classroom</t>
+  </si>
+  <si>
+    <t>https://training.play-with-docker.com/</t>
+  </si>
+  <si>
+    <t>Nơi thực hành Docker online</t>
+  </si>
+  <si>
+    <t>https://training.play-with-docker.com/ops-s1-hello/</t>
+  </si>
+  <si>
+    <t>Ở đây sẽ có 1 giao diện Command Line để thực hành Docker, ta cần phải đăng ký 1 Account trên Docker Hub để access vào giao diện Command Line đó</t>
+  </si>
+  <si>
+    <t>Hãy vào Docker Hub để đăng ký 1 account</t>
+  </si>
+  <si>
+    <t>https://hub.docker.com/</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dưới đây ta sẽ thực hành lệnh : </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>docker run hello-world</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,6 +208,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -208,7 +260,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
@@ -217,6 +269,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -230,6 +283,87 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>72</xdr:col>
+      <xdr:colOff>321298</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>107323</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="617220" y="1699260"/>
+          <a:ext cx="14517358" cy="7422523"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>67</xdr:col>
+      <xdr:colOff>1141</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>114896</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="617220" y="10294620"/>
+          <a:ext cx="13168501" cy="6881456"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -522,7 +656,7 @@
   <dimension ref="B2:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -541,7 +675,9 @@
       </c>
     </row>
     <row r="5" spans="2:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="B5" s="4"/>
+      <c r="B5" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -553,8 +689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -693,14 +829,265 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:H58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="72" width="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="B2" s="1"/>
+    </row>
+    <row r="4" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="B4" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="B5" s="4"/>
+      <c r="C5" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="F7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="F10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="F11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="F12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="F13" s="2"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="F14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="F15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="F16" s="2"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F17" s="2"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F18" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F20" s="2"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F21" s="2"/>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F22" s="2"/>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F23" s="2"/>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F24" s="2"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F25" s="2"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F26" s="2"/>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F27" s="2"/>
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F28" s="2"/>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F29" s="2"/>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F30" s="2"/>
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F31" s="2"/>
+      <c r="H31" s="2"/>
+    </row>
+    <row r="32" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F32" s="2"/>
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F33" s="2"/>
+      <c r="H33" s="2"/>
+    </row>
+    <row r="34" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F34" s="2"/>
+      <c r="H34" s="2"/>
+    </row>
+    <row r="35" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F35" s="2"/>
+      <c r="H35" s="2"/>
+    </row>
+    <row r="36" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F36" s="2"/>
+      <c r="H36" s="2"/>
+    </row>
+    <row r="37" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F37" s="2"/>
+      <c r="H37" s="2"/>
+    </row>
+    <row r="38" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F38" s="2"/>
+      <c r="H38" s="2"/>
+    </row>
+    <row r="39" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F39" s="2"/>
+      <c r="H39" s="2"/>
+    </row>
+    <row r="40" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F40" s="2"/>
+      <c r="H40" s="2"/>
+    </row>
+    <row r="41" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F41" s="2"/>
+      <c r="H41" s="2"/>
+    </row>
+    <row r="42" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F42" s="2"/>
+      <c r="H42" s="2"/>
+    </row>
+    <row r="43" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F43" s="2"/>
+      <c r="H43" s="2"/>
+    </row>
+    <row r="44" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F44" s="2"/>
+      <c r="H44" s="2"/>
+    </row>
+    <row r="45" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F45" s="2"/>
+      <c r="H45" s="2"/>
+    </row>
+    <row r="46" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F46" s="2"/>
+      <c r="H46" s="2"/>
+    </row>
+    <row r="47" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F47" s="2"/>
+      <c r="H47" s="2"/>
+    </row>
+    <row r="48" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F48" s="2"/>
+      <c r="H48" s="2"/>
+    </row>
+    <row r="49" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="F49" s="2"/>
+      <c r="H49" s="2"/>
+    </row>
+    <row r="50" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="F50" s="2"/>
+      <c r="H50" s="2"/>
+    </row>
+    <row r="51" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="F51" s="2"/>
+      <c r="H51" s="2"/>
+    </row>
+    <row r="52" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="F52" s="2"/>
+      <c r="H52" s="2"/>
+    </row>
+    <row r="53" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="F53" s="2"/>
+      <c r="H53" s="2"/>
+    </row>
+    <row r="54" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="F54" s="2"/>
+      <c r="H54" s="2"/>
+    </row>
+    <row r="55" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="F55" s="2"/>
+      <c r="H55" s="2"/>
+    </row>
+    <row r="56" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C56" t="s">
+        <v>22</v>
+      </c>
+      <c r="F56" s="2"/>
+      <c r="H56" s="2"/>
+    </row>
+    <row r="57" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C57" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="58" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D58" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C5" r:id="rId1"/>
+    <hyperlink ref="C8" r:id="rId2"/>
+    <hyperlink ref="D58" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
03. Docker Image, Docker Container, Docker Registry 04. Demo Gradle+SpringBoot_staging
</commit_message>
<xml_diff>
--- a/00. Huong dan Docker.xlsx
+++ b/00. Huong dan Docker.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
     <sheet name="01" sheetId="2" r:id="rId2"/>
     <sheet name="02" sheetId="4" r:id="rId3"/>
+    <sheet name="03" sheetId="5" r:id="rId4"/>
+    <sheet name="04" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="60">
   <si>
     <t>Sharing Docker dành cho Liên - Hiếu - Thảo</t>
   </si>
@@ -152,12 +154,199 @@
       <t>docker run hello-world</t>
     </r>
   </si>
+  <si>
+    <t>03 : Docker Image, Docker Container, Docker Registry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trang tham khảo : </t>
+  </si>
+  <si>
+    <t>https://xuanthulab.net/gioi-thieu-ve-docker-lam-quen-voi-docker-tao-container.html</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC22C72"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>image</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF212529"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t> là một gói phần mềm trong đó chứa những thứ cần như thư viện, các file cấu hình, biến môi trường để chạy mội ứng dụng nào đó.</t>
+    </r>
+  </si>
+  <si>
+    <t>Nó giống như cái USB chứa bộ cài đặt hệ điều hành Windows!</t>
+  </si>
+  <si>
+    <t>image trong Docker</t>
+  </si>
+  <si>
+    <t>container trong Docker</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Khi một phiên bản của image chạy, phiên bản chạy đó gọi là </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>container</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - (vậy muốn có container phải có image). Bất ký lúc nào bạn cũng có thể kiểm tra xem có bao nhiêu container đang chạy và nó sinh ra từ image nào.</t>
+    </r>
+  </si>
+  <si>
+    <t>(có thể xem image giống như file Ghost)</t>
+  </si>
+  <si>
+    <t>(có thể xem container giống như 1 máy tính đã được bung ghost, nó sẽ có các trạng thái gồm stop/running/…)</t>
+  </si>
+  <si>
+    <t>docker images -a</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> =&gt; Liệt kê danh sách các Docker Images trên hệ thống localhost</t>
+  </si>
+  <si>
+    <t>docker ps</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> =&gt; Liệt kê danh sách các container đang running</t>
+  </si>
+  <si>
+    <t>docker ps -a</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> =&gt; Liệt kê danh sách các tất cả container trong hệ thống (stop + running)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Server lưu trữ các image được gọi là Docker Registry. </t>
+  </si>
+  <si>
+    <t>Hiện tại dịch vụ Docker đã tạo sẵn 1 Docker Registry là Docker Hub (https://hub.docker.com/)</t>
+  </si>
+  <si>
+    <t>Ở đây đang chứa rất nhiều public images (Official Images + Sharing Images)</t>
+  </si>
+  <si>
+    <t>Giả sử ta cần deploy 1 project Java chạy Spring Boot + Gradle</t>
+  </si>
+  <si>
+    <t>Project đã được dev ngon lành và cung cấp các URL sau :</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/welcome</t>
+  </si>
+  <si>
+    <t>04. Demo Gradle+SpringBoot_staging</t>
+  </si>
+  <si>
+    <t>http://localhost:8080</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/dashboard</t>
+  </si>
+  <si>
+    <t>Cách chạy Docker</t>
+  </si>
+  <si>
+    <t>Vào folder /04. Gradle+SpringBoot_staging</t>
+  </si>
+  <si>
+    <t>Chạy lệnh sau</t>
+  </si>
+  <si>
+    <t>docker-compose up</t>
+  </si>
+  <si>
+    <t>Các bước sau đây đã diễn ra</t>
+  </si>
+  <si>
+    <t>Lưu ý trong vd này</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">File </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dockerfile</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> dùng để tạo 1 custom image mới từ 1 image có sẵn</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">File </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>docker-compose.yaml</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> dùng biên tập lệnh tương tác vào hệ thống Docker</t>
+    </r>
+  </si>
+  <si>
+    <t>03. Docker Image, Docker Container, Docker Registry</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -223,6 +412,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFC22C72"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF212529"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC22C72"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -260,7 +482,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
@@ -270,6 +492,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -355,6 +580,49 @@
         <a:xfrm>
           <a:off x="617220" y="10294620"/>
           <a:ext cx="13168501" cy="6881456"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>68</xdr:col>
+      <xdr:colOff>115469</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>114817</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="617220" y="5684520"/>
+          <a:ext cx="13488569" cy="5966977"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -653,10 +921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B5"/>
+  <dimension ref="B2:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -678,6 +946,61 @@
       <c r="B5" s="4" t="s">
         <v>18</v>
       </c>
+    </row>
+    <row r="6" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="B6" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="B7" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="B8" s="4"/>
+    </row>
+    <row r="9" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="B9" s="4"/>
+    </row>
+    <row r="10" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="B10" s="4"/>
+    </row>
+    <row r="11" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="B11" s="4"/>
+    </row>
+    <row r="12" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="B12" s="4"/>
+    </row>
+    <row r="13" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="B13" s="4"/>
+    </row>
+    <row r="14" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="B14" s="4"/>
+    </row>
+    <row r="15" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="B15" s="4"/>
+    </row>
+    <row r="16" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="B16" s="4"/>
+    </row>
+    <row r="17" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="B17" s="4"/>
+    </row>
+    <row r="18" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="B18" s="4"/>
+    </row>
+    <row r="19" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="B19" s="4"/>
+    </row>
+    <row r="20" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="B20" s="4"/>
+    </row>
+    <row r="21" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="B21" s="4"/>
+    </row>
+    <row r="22" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="B22" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -831,8 +1154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AE7" sqref="AE7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1090,4 +1413,255 @@
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
   <drawing r:id="rId5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:I28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="72" width="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="B2" s="1"/>
+    </row>
+    <row r="4" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B4" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B5" s="4"/>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="2:9" ht="15" x14ac:dyDescent="0.35">
+      <c r="D7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="F10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="E11" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="F13" s="2"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="F14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C15" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="E19" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="E22" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I5" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <drawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:H23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="72" width="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="B2" s="1"/>
+    </row>
+    <row r="4" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="B4" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="B5" s="4"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D10" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="F15" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D8" r:id="rId1"/>
+    <hyperlink ref="D9" r:id="rId2"/>
+    <hyperlink ref="D10" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
04. Demo Gradle+SpringBoot_staging 05. MySQL+Plain
</commit_message>
<xml_diff>
--- a/00. Huong dan Docker.xlsx
+++ b/00. Huong dan Docker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="02" sheetId="4" r:id="rId3"/>
     <sheet name="03" sheetId="5" r:id="rId4"/>
     <sheet name="04" sheetId="6" r:id="rId5"/>
+    <sheet name="05" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="79">
   <si>
     <t>Sharing Docker dành cho Liên - Hiếu - Thảo</t>
   </si>
@@ -522,6 +523,43 @@
   </si>
   <si>
     <t>Cuối cùng, ta sẽ test được các url  ở trên</t>
+  </si>
+  <si>
+    <t>05. MySQL+Plain</t>
+  </si>
+  <si>
+    <t>Tìm hiểu về Docker Compose</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Toàn bộ kịch bản tự động cho Docker có thể được viết trong file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>docker-compose.yml</t>
+    </r>
+  </si>
+  <si>
+    <t>Để chạy kịch bản trên, ta gọi lệnh</t>
+  </si>
+  <si>
+    <t>Tham khảo cách dựng MySQL DB Server bằng cách dùng Docker Compose</t>
+  </si>
+  <si>
+    <t>https://docs.docker.com/compose/</t>
+  </si>
+  <si>
+    <t>https://hub.docker.com/_/mysql</t>
+  </si>
+  <si>
+    <t>Ngoài ra, ta có thể chạy thử nghiệm Online với Docker Classroom</t>
   </si>
 </sst>
 </file>
@@ -834,6 +872,49 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>114880</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>76650</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="617220" y="2659380"/>
+          <a:ext cx="6698560" cy="5197290"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1123,8 +1204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1158,7 +1239,9 @@
       </c>
     </row>
     <row r="8" spans="2:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="B8" s="4"/>
+      <c r="B8" s="4" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="9" spans="2:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B9" s="4"/>
@@ -1210,10 +1293,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J24"/>
+  <dimension ref="B2:J27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1298,45 +1381,55 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:10" x14ac:dyDescent="0.3">
       <c r="H17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:10" x14ac:dyDescent="0.3">
       <c r="I18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:10" x14ac:dyDescent="0.3">
       <c r="I19" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:10" x14ac:dyDescent="0.3">
       <c r="J20" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:10" x14ac:dyDescent="0.3">
       <c r="J21" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:10" x14ac:dyDescent="0.3">
       <c r="G22" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="7:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G23" t="s">
         <v>6</v>
       </c>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="7:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H24" s="3" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="D27" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1345,6 +1438,7 @@
     <hyperlink ref="H14" r:id="rId2"/>
     <hyperlink ref="J20" r:id="rId3"/>
     <hyperlink ref="J21" r:id="rId4"/>
+    <hyperlink ref="D27" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1763,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AP33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1919,4 +2013,76 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:M12"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="72" width="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:13" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="B2" s="1"/>
+    </row>
+    <row r="4" spans="2:13" ht="18" x14ac:dyDescent="0.35">
+      <c r="B4" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" ht="18" x14ac:dyDescent="0.35">
+      <c r="B5" s="4"/>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="M6" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" ht="18" x14ac:dyDescent="0.35">
+      <c r="E9" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="E12" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="M6" r:id="rId1"/>
+    <hyperlink ref="E12" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <drawing r:id="rId4"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Delete 06 + 07
</commit_message>
<xml_diff>
--- a/00. Huong dan Docker.xlsx
+++ b/00. Huong dan Docker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,14 @@
     <sheet name="03" sheetId="5" r:id="rId4"/>
     <sheet name="04" sheetId="6" r:id="rId5"/>
     <sheet name="05" sheetId="7" r:id="rId6"/>
+    <sheet name="06" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="81">
   <si>
     <t>Sharing Docker dành cho Liên - Hiếu - Thảo</t>
   </si>
@@ -560,6 +561,12 @@
   </si>
   <si>
     <t>Ngoài ra, ta có thể chạy thử nghiệm Online với Docker Classroom</t>
+  </si>
+  <si>
+    <t>06. MySQL+PersistData</t>
+  </si>
+  <si>
+    <t>Sử dụng cơ chế volume để lưu giữ lại toàn bộ các files/folders trong MySQL từ bên trong container ra ngoài FileSystem của Windows/MacOS/Linux</t>
   </si>
 </sst>
 </file>
@@ -1204,8 +1211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1244,7 +1251,9 @@
       </c>
     </row>
     <row r="9" spans="2:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="B9" s="4"/>
+      <c r="B9" s="4" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="10" spans="2:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B10" s="4"/>
@@ -2019,7 +2028,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M12"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
@@ -2085,4 +2094,49 @@
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
   <drawing r:id="rId4"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="72" width="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="B2" s="1"/>
+    </row>
+    <row r="4" spans="2:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="B4" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E7" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E7" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
06. MySQL5.7+PersistData > Add SQL scripts
</commit_message>
<xml_diff>
--- a/00. Huong dan Docker.xlsx
+++ b/00. Huong dan Docker.xlsx
@@ -932,14 +932,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>47</xdr:col>
-      <xdr:colOff>69335</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>145236</xdr:rowOff>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>76813</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>152841</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -953,7 +953,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1028700" y="2202180"/>
-          <a:ext cx="8710415" cy="5265876"/>
+          <a:ext cx="7071973" cy="5090601"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2072,7 +2072,7 @@
   <dimension ref="B2:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2143,8 +2143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
07. SpringBoot+MySQL5.7 + 08. SpringBoot+MySQL5.7_Networks
</commit_message>
<xml_diff>
--- a/00. Huong dan Docker.xlsx
+++ b/00. Huong dan Docker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -14,13 +14,15 @@
     <sheet name="04" sheetId="6" r:id="rId5"/>
     <sheet name="05" sheetId="7" r:id="rId6"/>
     <sheet name="06" sheetId="9" r:id="rId7"/>
+    <sheet name="07" sheetId="11" r:id="rId8"/>
+    <sheet name="08" sheetId="12" r:id="rId9"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="102">
   <si>
     <t>Sharing Docker dành cho Liên - Hiếu - Thảo</t>
   </si>
@@ -567,13 +569,99 @@
   </si>
   <si>
     <t>Sử dụng cơ chế volume để lưu giữ lại toàn bộ các files/folders trong MySQL từ bên trong container ra ngoài FileSystem của Windows/MacOS/Linux</t>
+  </si>
+  <si>
+    <t>07. SpringBoot+MySQL5.7</t>
+  </si>
+  <si>
+    <t>Dựng 1 service Java (dạng SpringBoot) + 1 Service MySQL 5.7</t>
+  </si>
+  <si>
+    <t>Tìm hiểu các khái niệm sau đây</t>
+  </si>
+  <si>
+    <t>Biến môi trường trong docker-compose.yaml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      MYSQL_SERVER: mysql_db_jpa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      MYSQL_SERVER_PORT: 3306</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      MYSQL_USER: root</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      MYSQL_PASSWORD: root</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      APP_SERVER_PORT: 9222</t>
+  </si>
+  <si>
+    <t>Các service trong cùng file docker-compose mặc định hiểu được nhau (cùng network)</t>
+  </si>
+  <si>
+    <t>https://docs.docker.com/compose/environment-variables/</t>
+  </si>
+  <si>
+    <t>mysql_db_jpa</t>
+  </si>
+  <si>
+    <t>gradle_spring_boot</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tìm hiểu khái niệm </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>depends_on</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, lúc đó thứ tự chạy service sẽ như sau :</t>
+    </r>
+  </si>
+  <si>
+    <t>https://docs.docker.com/compose/compose-file/</t>
+  </si>
+  <si>
+    <t>08. SpringBoot+MySQL5.7_Networks</t>
+  </si>
+  <si>
+    <t>Dựng 1 service Java (dạng SpringBoot) + 1 Service MySQL 5.7 + Các service MySQL khác</t>
+  </si>
+  <si>
+    <t>và có phân nhóm sử dụng các networks khác nhau trong Docker</t>
+  </si>
+  <si>
+    <t>https://docs.docker.com/network/</t>
+  </si>
+  <si>
+    <t>Các services nằm trong cùng 1 file Docker Compose mặc định thuộc chung 1 network</t>
+  </si>
+  <si>
+    <t>Nếu ta chỉ định network cho các service thì các service cùng chung network mới hiểu được nhau</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -684,6 +772,14 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -954,6 +1050,130 @@
         <a:xfrm>
           <a:off x="1028700" y="2202180"/>
           <a:ext cx="7071973" cy="5090601"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>38642</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>122485</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="982980" y="3307080"/>
+          <a:ext cx="6256562" cy="6515665"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>45</xdr:col>
+      <xdr:colOff>54057</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>107095</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1036320" y="11597640"/>
+          <a:ext cx="8276037" cy="4793395"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>23397</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>84366</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="822960" y="2567940"/>
+          <a:ext cx="6195597" cy="6302286"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2143,8 +2363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AO4" sqref="AO4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2183,4 +2403,180 @@
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <drawing r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F62"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AT57" sqref="AT57"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="72" width="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="B2" s="1"/>
+    </row>
+    <row r="4" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="B4" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E15" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E18" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="58" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E58" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="59" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="F59" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="60" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="F60" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="62" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E62" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E15" r:id="rId1"/>
+    <hyperlink ref="E62" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <drawing r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="72" width="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="B2" s="1"/>
+    </row>
+    <row r="4" spans="2:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="B4" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D9" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E17" s="2"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D9" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <drawing r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
10. Mockaroo & 11. Jenkins
</commit_message>
<xml_diff>
--- a/00. Huong dan Docker.xlsx
+++ b/00. Huong dan Docker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="9"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -17,13 +17,15 @@
     <sheet name="07" sheetId="11" r:id="rId8"/>
     <sheet name="08" sheetId="12" r:id="rId9"/>
     <sheet name="09" sheetId="13" r:id="rId10"/>
+    <sheet name="10" sheetId="15" r:id="rId11"/>
+    <sheet name="11" sheetId="16" r:id="rId12"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="139">
   <si>
     <t>Sharing Docker dành cho Liên - Hiếu - Thảo</t>
   </si>
@@ -713,6 +715,60 @@
   </si>
   <si>
     <t>http://wiremock.org/docs/response-templating/</t>
+  </si>
+  <si>
+    <t>10. Mockaroo</t>
+  </si>
+  <si>
+    <t>Sử dụng Mockaroo để tạo ra các bộ data test dạng table với nhiều format khác nhau</t>
+  </si>
+  <si>
+    <t>https://www.mockaroo.com/</t>
+  </si>
+  <si>
+    <t>11. Jenkins</t>
+  </si>
+  <si>
+    <t>Dựng nền tảng Jenkins bằng Docker</t>
+  </si>
+  <si>
+    <t>https://blog.arrow-tech.vn/continuous-integration-voi-jenkins-docker/</t>
+  </si>
+  <si>
+    <t>Continuous Integration với Jenkins &amp; Docker (P1)</t>
+  </si>
+  <si>
+    <t>Account Information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UserName </t>
+  </si>
+  <si>
+    <t>thaochau</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>root</t>
+  </si>
+  <si>
+    <t>Full Name</t>
+  </si>
+  <si>
+    <t>Thao Chau</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>thaochau@gmail.com</t>
+  </si>
+  <si>
+    <t>Docker Hub</t>
+  </si>
+  <si>
+    <t>https://hub.docker.com/r/jenkinsci/blueocean</t>
   </si>
 </sst>
 </file>
@@ -1715,6 +1771,49 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>45</xdr:col>
+      <xdr:colOff>115059</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>130122</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="617220" y="1653540"/>
+          <a:ext cx="8756139" cy="6713802"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2097,8 +2196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AP34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AM35" sqref="AM35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2301,6 +2400,147 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>
   <drawing r:id="rId9"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="72" width="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="B2" s="1"/>
+    </row>
+    <row r="4" spans="2:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="B4" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D7" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D9" s="2"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D7" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <drawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:I19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S17" sqref="S17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="72" width="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="B2" s="1"/>
+    </row>
+    <row r="4" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B4" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D10" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D13" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E16" t="s">
+        <v>129</v>
+      </c>
+      <c r="I16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E17" t="s">
+        <v>131</v>
+      </c>
+      <c r="I17" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E18" t="s">
+        <v>133</v>
+      </c>
+      <c r="I18" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="19" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E19" t="s">
+        <v>135</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D10" r:id="rId1"/>
+    <hyperlink ref="I19" r:id="rId2"/>
+    <hyperlink ref="D13" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>